<commit_message>
added check for duplicate order, added discord webhook when checkout
</commit_message>
<xml_diff>
--- a/asins.xlsx
+++ b/asins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Olazabal\Desktop\amazonBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A689A9-772E-4217-910E-2FE71DAD52F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3803AA38-9918-41D5-923A-E8B5B2EB70F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9396" yWindow="3000" windowWidth="13704" windowHeight="6084" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
+    <workbookView xWindow="9396" yWindow="3000" windowWidth="15648" windowHeight="9888" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ASIN</t>
   </si>
@@ -81,10 +81,16 @@
     <t>B0815Y8J9N</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>B08166SLDF</t>
+  </si>
+  <si>
+    <t>5600x</t>
+  </si>
+  <si>
+    <t>5800x</t>
+  </si>
+  <si>
+    <t>B0815XFSGK</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F9F030-38C1-49B3-A723-745FF1F78A76}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,13 +544,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8">
         <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed signin to be the first step
</commit_message>
<xml_diff>
--- a/asins.xlsx
+++ b/asins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Olazabal\Desktop\amazonBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorolazabal/Desktop/amazonBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3803AA38-9918-41D5-923A-E8B5B2EB70F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770317BD-7969-FA4D-83BE-823AAF7C52D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9396" yWindow="3000" windowWidth="15648" windowHeight="9888" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
+    <workbookView xWindow="9400" yWindow="3000" windowWidth="15640" windowHeight="9880" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ASIN</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>B0815XFSGK</t>
+  </si>
+  <si>
+    <t>B08L8KC1J7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASUS TUF Gaming NVIDIA GeForce RTX 3070 OC Edition </t>
   </si>
 </sst>
 </file>
@@ -452,20 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F9F030-38C1-49B3-A723-745FF1F78A76}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="1" max="1" width="40.5" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -476,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -487,7 +493,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -498,7 +504,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -509,58 +515,69 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>640</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>425</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed some bugs and more good things
</commit_message>
<xml_diff>
--- a/asins.xlsx
+++ b/asins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorolazabal/Desktop/amazonBot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Olazabal\Desktop\amazonBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770317BD-7969-FA4D-83BE-823AAF7C52D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B39372-B4DC-4A52-B7A6-E7EFAF2A6BF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="3000" windowWidth="15640" windowHeight="9880" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
+    <workbookView xWindow="9396" yWindow="3000" windowWidth="15648" windowHeight="9888" xr2:uid="{808BC00B-ECDB-4119-A19B-40CB9DAE7945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ASIN</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t xml:space="preserve">ASUS TUF Gaming NVIDIA GeForce RTX 3070 OC Edition </t>
+  </si>
+  <si>
+    <t>B08HH5WF97</t>
+  </si>
+  <si>
+    <t>ASUS TUF Gaming NVIDIA GeForce RTX 3080</t>
+  </si>
+  <si>
+    <t>B08HR3Y5GQ</t>
+  </si>
+  <si>
+    <t>EVGA 10G-P5-3897-KR GeForce RTX 3080 FTW3 ULTRA</t>
+  </si>
+  <si>
+    <t>B08J6F174Z</t>
+  </si>
+  <si>
+    <t>ASUS ROG STRIX NVIDIA GeForce RTX 3080</t>
   </si>
 </sst>
 </file>
@@ -458,20 +476,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F9F030-38C1-49B3-A723-745FF1F78A76}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.5" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -482,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -493,7 +511,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -504,7 +522,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -515,7 +533,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -526,7 +544,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -537,47 +555,80 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>800</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>425</v>
       </c>
     </row>

</xml_diff>